<commit_message>
add new  metrics -> peaks article
</commit_message>
<xml_diff>
--- a/Peaks-dataset-article/Teste00/content/results/metrics_1_1.xlsx
+++ b/Peaks-dataset-article/Teste00/content/results/metrics_1_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,79 +484,640 @@
           <t>mse_vt</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>mape</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>rmse</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>r2_adj</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>rsd</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>aic</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>bic</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>model_1_1_1</t>
+          <t>model_1_1_10</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8519678385072635</v>
+        <v>0.4953326578859717</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7621175696959096</v>
+        <v>0.3928119398570212</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8707586959922051</v>
+        <v>0.2310542050459409</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.4108597960044833</v>
+        <v>-1.119295537393047</v>
       </c>
       <c r="F2" t="n">
-        <v>0.76472228219772</v>
+        <v>0.2644810755410532</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2101101646993679</v>
+        <v>0.7163020339682984</v>
       </c>
       <c r="H2" t="n">
-        <v>0.3376395784961284</v>
+        <v>0.8618153111706797</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3363248578140017</v>
+        <v>0.5616035936284579</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3330643877578196</v>
+        <v>0.3952555833329181</v>
       </c>
       <c r="K2" t="n">
-        <v>0.3346946307256673</v>
+        <v>0.4784296272356043</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2.230345491166361</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.8463462849025205</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1.006980989170453</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.8823769984291556</v>
+      </c>
+      <c r="P2" t="n">
+        <v>3518.667306731636</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>5662.6698826748</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
+          <t>model_1_1_9</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.4855896727212997</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.3843036647841478</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.2227034348707476</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1.166483453607337</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.2530279522092613</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.7301307871052523</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.8738915725644354</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.5677026224166107</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.4040562848020897</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.4858794879313618</v>
+      </c>
+      <c r="L3" t="n">
+        <v>2.252789527778963</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.8544769084681295</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1.00711576245227</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.8908537594726637</v>
+      </c>
+      <c r="P3" t="n">
+        <v>3518.629063200938</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>5662.631639144102</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>model_1_1_8</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.4756228050753467</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.3755867535778571</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.2140027867738743</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-1.215144325183455</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.2411672306773459</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.7442773089253145</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.8862639626636868</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.5740571863795915</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.4131316972874887</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.4935944771621744</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2.275478841211165</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.8627150798063719</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1.007253632667546</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.8994426468201406</v>
+      </c>
+      <c r="P4" t="n">
+        <v>3518.590683173089</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>5662.593259116254</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>model_1_1_7</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.4654273160933792</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.3666563143727104</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.2049421372892146</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1.265312682743204</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.2288883364312014</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.7587483255448814</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.8989394247613144</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.5806746792439574</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.4224882608635745</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.501581473283817</v>
+      </c>
+      <c r="L5" t="n">
+        <v>2.298416815285488</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.8710616083520621</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1.007394665368161</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.9081445043657169</v>
+      </c>
+      <c r="P5" t="n">
+        <v>3518.552170286942</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>5662.554746230107</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>model_1_1_6</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.454998642184853</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.3575077652838905</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1955107197190499</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-1.317012082575049</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.2161818394213789</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.7735503143182734</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.9119244621777038</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.5875629645238472</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.4321303688555698</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5098466102173793</v>
+      </c>
+      <c r="L6" t="n">
+        <v>2.321600024286796</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.8795170915441458</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1.007538923681593</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.9169599549825508</v>
+      </c>
+      <c r="P6" t="n">
+        <v>3518.51352912697</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>5662.516105070134</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>model_1_1_5</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.4443316226854355</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.3481358705493798</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.1857004112493189</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-1.370276066626338</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.2030381386098357</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.7886906000593821</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.9252265063170094</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.5947279747591053</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.4420642769468995</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.518396133106119</v>
+      </c>
+      <c r="L7" t="n">
+        <v>2.3450356913896</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.8880825412423003</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1.007686478994553</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.9258900536072809</v>
+      </c>
+      <c r="P7" t="n">
+        <v>3518.474762353841</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>5662.477338297006</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>model_1_1_4</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.4334219372628492</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.3385358301339693</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.1755008577190638</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-1.42513465729099</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.1894474190972321</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.8041753148527303</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.9388523701324307</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.6021772721654841</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.4522955844127053</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.5272364262026721</v>
+      </c>
+      <c r="L8" t="n">
+        <v>2.368721880658982</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.8967582254168235</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1.007837391069563</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.9349350796182555</v>
+      </c>
+      <c r="P8" t="n">
+        <v>3518.435875960548</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>5662.438451903712</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>model_1_1_3</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.4222636193354706</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.3287022391259303</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.1649009530845241</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-1.481618444878248</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.1753989550772675</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.820012927394816</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.9528097251115828</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.6099189681002828</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.4628299964462045</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.5363744662731551</v>
+      </c>
+      <c r="L9" t="n">
+        <v>2.392666272516194</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.9055456517452977</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1.007991742441469</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.9440966048780132</v>
+      </c>
+      <c r="P9" t="n">
+        <v>3518.396870347465</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>5662.399446290629</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>model_1_1_2</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.4108515558629828</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.3186297807598635</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.1538909495948987</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-1.539766740999173</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.1608815195870662</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.8362106949041537</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.9671061176311615</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.6179601818844156</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.4736748447920674</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.5458175560687075</v>
+      </c>
+      <c r="L10" t="n">
+        <v>2.416867143407515</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.9144455669443391</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1.008149603838207</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.9533754078924419</v>
+      </c>
+      <c r="P10" t="n">
+        <v>3518.357749340507</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>5662.360325283672</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>model_1_1_1</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.3991810324186368</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.3083136229521977</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.1424621652881335</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-1.599602061898369</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.1458873258403255</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.8527753088251608</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.9817484061323647</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.6263072544343959</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.4848343288039179</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.5555707606245639</v>
+      </c>
+      <c r="L11" t="n">
+        <v>2.441322816673428</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.9234583416836738</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1.008311040473748</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.9627718751114459</v>
+      </c>
+      <c r="P11" t="n">
+        <v>3518.318518358112</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>5662.321094301276</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
           <t>model_1_1_0</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>0.850409805267425</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.7605423523757331</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.870912396056134</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-0.4157223269792187</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.7644593903462179</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.2123215667172032</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.3398753708215401</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.3359248838850499</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.3342122948047425</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.335068607879055</v>
+      <c r="B12" t="n">
+        <v>0.3872466315611516</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.2977482218810343</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.130603839229409</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-1.661154602506695</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.1304055051526124</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.8697144584293335</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.9967444592656287</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.6349680450553987</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.4963140799356048</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.5656411496441254</v>
+      </c>
+      <c r="L12" t="n">
+        <v>2.466041312637266</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.9325848263988287</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1.008476127286762</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.9722868931753528</v>
+      </c>
+      <c r="P12" t="n">
+        <v>3518.279180659815</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>5662.28175660298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>